<commit_message>
Fix AP 2 & AP DeepSTL 1
</commit_message>
<xml_diff>
--- a/script/result_llm_tranform/ardupilot_docs/ap_follow-mode/result.xlsx
+++ b/script/result_llm_tranform/ardupilot_docs/ap_follow-mode/result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19464" windowHeight="9024"/>
+    <workbookView windowWidth="12035" windowHeight="9024"/>
   </bookViews>
   <sheets>
     <sheet name="mtl" sheetId="1" r:id="rId1"/>
@@ -1279,8 +1279,8 @@
   <sheetPr/>
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>